<commit_message>
working through errors. C and C2 are mixed up sometimes which leads to error in operational days. Issue is that day observed is after the camera allegedly stopped working or the observation is after the camera was removed (the former is the most common not the latter).
</commit_message>
<xml_diff>
--- a/2014/OperationsDays2014_work.xlsx
+++ b/2014/OperationsDays2014_work.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elise/Desktop/MP/Belize-MP-Bruno-Boos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elise/Desktop/MP/Belize-MP-Bruno-Boos/2014/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00021FC9-FB4C-9E44-91A9-AE63793C7E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204B657F-42C4-9A4E-865D-55D398FC8586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1400" windowWidth="27240" windowHeight="15560" activeTab="2" xr2:uid="{35824555-D2CA-254A-AC41-7E00E7980052}"/>
+    <workbookView xWindow="10240" yWindow="640" windowWidth="27240" windowHeight="15560" activeTab="2" xr2:uid="{35824555-D2CA-254A-AC41-7E00E7980052}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="OperationsDays2014" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="96">
   <si>
     <t>401A</t>
   </si>
@@ -320,6 +321,12 @@
   </si>
   <si>
     <t>December 22, 2014</t>
+  </si>
+  <si>
+    <t>removeday</t>
+  </si>
+  <si>
+    <t>Date Removed</t>
   </si>
 </sst>
 </file>
@@ -328,7 +335,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -366,13 +373,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2286,7 +2294,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{945E4251-CA6D-704A-ACF6-9BC71BB06730}">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
@@ -2294,10 +2302,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="17.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.83203125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>82</v>
       </c>
@@ -2313,8 +2321,11 @@
       <c r="E1" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2330,8 +2341,11 @@
       <c r="E2" s="5">
         <v>41716</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="5">
+        <v>41752</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2347,8 +2361,11 @@
       <c r="E3" s="5">
         <v>41752</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -2364,8 +2381,11 @@
       <c r="E4" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -2381,8 +2401,11 @@
       <c r="E5" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="5">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
@@ -2398,8 +2421,11 @@
       <c r="E6" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
@@ -2415,8 +2441,11 @@
       <c r="E7" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="5">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>42</v>
       </c>
@@ -2432,8 +2461,11 @@
       <c r="E8" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>53</v>
       </c>
@@ -2449,8 +2481,11 @@
       <c r="E9" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="5">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>63</v>
       </c>
@@ -2466,8 +2501,11 @@
       <c r="E10" s="5">
         <v>41995</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="5">
+        <v>42053</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -2483,8 +2521,11 @@
       <c r="E11" s="5">
         <v>41716</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="5">
+        <v>41752</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -2500,8 +2541,11 @@
       <c r="E12" s="5">
         <v>41752</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -2517,8 +2561,11 @@
       <c r="E13" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>32</v>
       </c>
@@ -2534,8 +2581,11 @@
       <c r="E14" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="5">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>43</v>
       </c>
@@ -2551,8 +2601,11 @@
       <c r="E15" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>54</v>
       </c>
@@ -2568,8 +2621,11 @@
       <c r="E16" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="5">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>64</v>
       </c>
@@ -2585,8 +2641,11 @@
       <c r="E17" s="5">
         <v>41995</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="5">
+        <v>42053</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
@@ -2602,8 +2661,11 @@
       <c r="E18" s="5">
         <v>41752</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
@@ -2619,8 +2681,11 @@
       <c r="E19" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>33</v>
       </c>
@@ -2636,8 +2701,11 @@
       <c r="E20" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="5">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>44</v>
       </c>
@@ -2653,8 +2721,11 @@
       <c r="E21" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>55</v>
       </c>
@@ -2670,8 +2741,11 @@
       <c r="E22" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="5">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>65</v>
       </c>
@@ -2687,8 +2761,11 @@
       <c r="E23" s="5">
         <v>41995</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="5">
+        <v>42053</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
@@ -2704,8 +2781,11 @@
       <c r="E24" s="5">
         <v>41716</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="5">
+        <v>41752</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>10</v>
       </c>
@@ -2721,8 +2801,11 @@
       <c r="E25" s="5">
         <v>41752</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>21</v>
       </c>
@@ -2738,8 +2821,11 @@
       <c r="E26" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>34</v>
       </c>
@@ -2755,8 +2841,11 @@
       <c r="E27" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="5">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>45</v>
       </c>
@@ -2772,8 +2861,11 @@
       <c r="E28" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>56</v>
       </c>
@@ -2789,8 +2881,11 @@
       <c r="E29" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="5">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>66</v>
       </c>
@@ -2806,8 +2901,11 @@
       <c r="E30" s="5">
         <v>41995</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" s="5">
+        <v>42053</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>3</v>
       </c>
@@ -2823,8 +2921,11 @@
       <c r="E31" s="5">
         <v>41716</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" s="5">
+        <v>41752</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>11</v>
       </c>
@@ -2840,8 +2941,11 @@
       <c r="E32" s="5">
         <v>41752</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>22</v>
       </c>
@@ -2857,8 +2961,11 @@
       <c r="E33" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>35</v>
       </c>
@@ -2874,8 +2981,11 @@
       <c r="E34" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="5">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>46</v>
       </c>
@@ -2891,8 +3001,11 @@
       <c r="E35" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>57</v>
       </c>
@@ -2908,8 +3021,11 @@
       <c r="E36" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" s="5">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>4</v>
       </c>
@@ -2925,8 +3041,11 @@
       <c r="E37" s="5">
         <v>41716</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" s="5">
+        <v>41752</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>12</v>
       </c>
@@ -2942,8 +3061,11 @@
       <c r="E38" s="5">
         <v>41752</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>23</v>
       </c>
@@ -2959,8 +3081,11 @@
       <c r="E39" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>36</v>
       </c>
@@ -2976,8 +3101,11 @@
       <c r="E40" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" s="5">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>47</v>
       </c>
@@ -2993,8 +3121,11 @@
       <c r="E41" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>58</v>
       </c>
@@ -3010,8 +3141,11 @@
       <c r="E42" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" s="5">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>67</v>
       </c>
@@ -3027,8 +3161,11 @@
       <c r="E43" s="5">
         <v>41995</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" s="5">
+        <v>42053</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>13</v>
       </c>
@@ -3044,8 +3181,11 @@
       <c r="E44" s="5">
         <v>41752</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>24</v>
       </c>
@@ -3061,8 +3201,11 @@
       <c r="E45" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>37</v>
       </c>
@@ -3078,8 +3221,11 @@
       <c r="E46" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" s="5">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>48</v>
       </c>
@@ -3095,8 +3241,11 @@
       <c r="E47" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>59</v>
       </c>
@@ -3112,8 +3261,11 @@
       <c r="E48" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" s="5">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>5</v>
       </c>
@@ -3129,8 +3281,11 @@
       <c r="E49" s="5">
         <v>41716</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" s="5">
+        <v>41752</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>14</v>
       </c>
@@ -3146,8 +3301,11 @@
       <c r="E50" s="5">
         <v>41752</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>25</v>
       </c>
@@ -3163,8 +3321,11 @@
       <c r="E51" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>38</v>
       </c>
@@ -3180,8 +3341,11 @@
       <c r="E52" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" s="5">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>49</v>
       </c>
@@ -3197,8 +3361,11 @@
       <c r="E53" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>60</v>
       </c>
@@ -3214,8 +3381,11 @@
       <c r="E54" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" s="5">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>68</v>
       </c>
@@ -3231,8 +3401,11 @@
       <c r="E55" s="5">
         <v>41995</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55" s="5">
+        <v>42053</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>6</v>
       </c>
@@ -3248,8 +3421,11 @@
       <c r="E56" s="5">
         <v>41716</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" s="5">
+        <v>41752</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>15</v>
       </c>
@@ -3265,8 +3441,11 @@
       <c r="E57" s="5">
         <v>41752</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>26</v>
       </c>
@@ -3282,8 +3461,11 @@
       <c r="E58" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>39</v>
       </c>
@@ -3299,8 +3481,11 @@
       <c r="E59" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59" s="5">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>50</v>
       </c>
@@ -3316,8 +3501,11 @@
       <c r="E60" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>16</v>
       </c>
@@ -3333,8 +3521,11 @@
       <c r="E61" s="5">
         <v>41752</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>27</v>
       </c>
@@ -3350,8 +3541,11 @@
       <c r="E62" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>69</v>
       </c>
@@ -3367,8 +3561,11 @@
       <c r="E63" s="5">
         <v>41995</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63" s="5">
+        <v>42053</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>17</v>
       </c>
@@ -3384,8 +3581,11 @@
       <c r="E64" s="5">
         <v>41752</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>28</v>
       </c>
@@ -3401,8 +3601,11 @@
       <c r="E65" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>51</v>
       </c>
@@ -3418,8 +3621,11 @@
       <c r="E66" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>61</v>
       </c>
@@ -3435,8 +3641,11 @@
       <c r="E67" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67" s="5">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>29</v>
       </c>
@@ -3452,8 +3661,11 @@
       <c r="E68" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>40</v>
       </c>
@@ -3469,8 +3681,11 @@
       <c r="E69" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69" s="5">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>52</v>
       </c>
@@ -3486,8 +3701,11 @@
       <c r="E70" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>62</v>
       </c>
@@ -3503,8 +3721,11 @@
       <c r="E71" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71" s="5">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>70</v>
       </c>
@@ -3519,6 +3740,9 @@
       </c>
       <c r="E72" s="5">
         <v>41995</v>
+      </c>
+      <c r="F72" s="5">
+        <v>42053</v>
       </c>
     </row>
   </sheetData>
@@ -4337,4 +4561,1037 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{505DB0B9-E048-0A4F-958B-1599B5D3CFCF}">
+  <dimension ref="A1:E72"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="4">
+        <v>41716</v>
+      </c>
+      <c r="D2" s="5">
+        <v>41752</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="4">
+        <v>41752</v>
+      </c>
+      <c r="D3" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="4">
+        <v>41787</v>
+      </c>
+      <c r="D4" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="4">
+        <v>41838</v>
+      </c>
+      <c r="D5" s="5">
+        <v>41900</v>
+      </c>
+      <c r="E5" s="6">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="4">
+        <v>41900</v>
+      </c>
+      <c r="D6" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="4">
+        <v>41838</v>
+      </c>
+      <c r="D7" s="5">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="4">
+        <v>41900</v>
+      </c>
+      <c r="D8" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="4">
+        <v>41946</v>
+      </c>
+      <c r="D9" s="5">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="5">
+        <v>42053</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="4">
+        <v>41716</v>
+      </c>
+      <c r="D11" s="5">
+        <v>41752</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="4">
+        <v>41752</v>
+      </c>
+      <c r="D12" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="4">
+        <v>41787</v>
+      </c>
+      <c r="D13" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="4">
+        <v>41838</v>
+      </c>
+      <c r="D14" s="5">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="4">
+        <v>41900</v>
+      </c>
+      <c r="D15" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="4">
+        <v>41946</v>
+      </c>
+      <c r="D16" s="5">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="5">
+        <v>42053</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="4">
+        <v>41752</v>
+      </c>
+      <c r="D18" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="4">
+        <v>41787</v>
+      </c>
+      <c r="D19" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="4">
+        <v>41838</v>
+      </c>
+      <c r="D20" s="5">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="4">
+        <v>41900</v>
+      </c>
+      <c r="D21" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="4">
+        <v>41946</v>
+      </c>
+      <c r="D22" s="5">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="5">
+        <v>42053</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="4">
+        <v>41716</v>
+      </c>
+      <c r="D24" s="5">
+        <v>41752</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="4">
+        <v>41752</v>
+      </c>
+      <c r="D25" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="4">
+        <v>41787</v>
+      </c>
+      <c r="D26" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="4">
+        <v>41838</v>
+      </c>
+      <c r="D27" s="5">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="4">
+        <v>41900</v>
+      </c>
+      <c r="D28" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="4">
+        <v>41946</v>
+      </c>
+      <c r="D29" s="5">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" s="5">
+        <v>42053</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="4">
+        <v>41716</v>
+      </c>
+      <c r="D31" s="5">
+        <v>41752</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="4">
+        <v>41752</v>
+      </c>
+      <c r="D32" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="4">
+        <v>41787</v>
+      </c>
+      <c r="D33" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="4">
+        <v>41838</v>
+      </c>
+      <c r="D34" s="5">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="4">
+        <v>41900</v>
+      </c>
+      <c r="D35" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="4">
+        <v>41946</v>
+      </c>
+      <c r="D36" s="5">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" s="4">
+        <v>41716</v>
+      </c>
+      <c r="D37" s="5">
+        <v>41752</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="4">
+        <v>41752</v>
+      </c>
+      <c r="D38" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="4">
+        <v>41787</v>
+      </c>
+      <c r="D39" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="4">
+        <v>41838</v>
+      </c>
+      <c r="D40" s="5">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="4">
+        <v>41900</v>
+      </c>
+      <c r="D41" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="4">
+        <v>41946</v>
+      </c>
+      <c r="D42" s="5">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" t="s">
+        <v>93</v>
+      </c>
+      <c r="D43" s="5">
+        <v>42053</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="4">
+        <v>41752</v>
+      </c>
+      <c r="D44" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" s="4">
+        <v>41787</v>
+      </c>
+      <c r="D45" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="4">
+        <v>41838</v>
+      </c>
+      <c r="D46" s="5">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" s="4">
+        <v>41900</v>
+      </c>
+      <c r="D47" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" s="4">
+        <v>41946</v>
+      </c>
+      <c r="D48" s="5">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" s="4">
+        <v>41716</v>
+      </c>
+      <c r="D49" s="5">
+        <v>41752</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" s="4">
+        <v>41752</v>
+      </c>
+      <c r="D50" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51" s="4">
+        <v>41787</v>
+      </c>
+      <c r="D51" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" s="4">
+        <v>41838</v>
+      </c>
+      <c r="D52" s="5">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" s="4">
+        <v>41900</v>
+      </c>
+      <c r="D53" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54" s="4">
+        <v>41946</v>
+      </c>
+      <c r="D54" s="5">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55" t="s">
+        <v>90</v>
+      </c>
+      <c r="C55" t="s">
+        <v>93</v>
+      </c>
+      <c r="D55" s="5">
+        <v>42053</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" t="s">
+        <v>90</v>
+      </c>
+      <c r="C56" s="4">
+        <v>41716</v>
+      </c>
+      <c r="D56" s="5">
+        <v>41752</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B57" t="s">
+        <v>90</v>
+      </c>
+      <c r="C57" s="4">
+        <v>41752</v>
+      </c>
+      <c r="D57" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" t="s">
+        <v>90</v>
+      </c>
+      <c r="C58" s="4">
+        <v>41787</v>
+      </c>
+      <c r="D58" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B59" t="s">
+        <v>90</v>
+      </c>
+      <c r="C59" s="4">
+        <v>41838</v>
+      </c>
+      <c r="D59" s="5">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B60" t="s">
+        <v>90</v>
+      </c>
+      <c r="C60" s="4">
+        <v>41900</v>
+      </c>
+      <c r="D60" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>16</v>
+      </c>
+      <c r="B61" t="s">
+        <v>92</v>
+      </c>
+      <c r="C61" s="4">
+        <v>41752</v>
+      </c>
+      <c r="D61" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" t="s">
+        <v>92</v>
+      </c>
+      <c r="C62" s="4">
+        <v>41787</v>
+      </c>
+      <c r="D62" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B63" t="s">
+        <v>92</v>
+      </c>
+      <c r="C63" t="s">
+        <v>93</v>
+      </c>
+      <c r="D63" s="5">
+        <v>42053</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>17</v>
+      </c>
+      <c r="B64" t="s">
+        <v>92</v>
+      </c>
+      <c r="C64" s="4">
+        <v>41752</v>
+      </c>
+      <c r="D64" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B65" t="s">
+        <v>92</v>
+      </c>
+      <c r="C65" s="4">
+        <v>41787</v>
+      </c>
+      <c r="D65" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B66" t="s">
+        <v>92</v>
+      </c>
+      <c r="C66" s="4">
+        <v>41900</v>
+      </c>
+      <c r="D66" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B67" t="s">
+        <v>92</v>
+      </c>
+      <c r="C67" s="4">
+        <v>41946</v>
+      </c>
+      <c r="D67" s="5">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B68" t="s">
+        <v>91</v>
+      </c>
+      <c r="C68" s="4">
+        <v>41787</v>
+      </c>
+      <c r="D68" s="5">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B69" t="s">
+        <v>91</v>
+      </c>
+      <c r="C69" s="4">
+        <v>41838</v>
+      </c>
+      <c r="D69" s="5">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B70" t="s">
+        <v>91</v>
+      </c>
+      <c r="C70" s="4">
+        <v>41900</v>
+      </c>
+      <c r="D70" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B71" t="s">
+        <v>92</v>
+      </c>
+      <c r="C71" s="4">
+        <v>41946</v>
+      </c>
+      <c r="D71" s="5">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>92</v>
+      </c>
+      <c r="C72" t="s">
+        <v>93</v>
+      </c>
+      <c r="D72" s="5">
+        <v>42053</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D72">
+    <sortCondition ref="A2:A72"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
working through C and C2 all but one figured out. Unsure about the ones that aren't the c's how they got screwy but will look at later
</commit_message>
<xml_diff>
--- a/2014/OperationsDays2014_work.xlsx
+++ b/2014/OperationsDays2014_work.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elise/Desktop/MP/Belize-MP-Bruno-Boos/2014/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204B657F-42C4-9A4E-865D-55D398FC8586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7697D4-2187-F143-8644-65593C70EFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10240" yWindow="640" windowWidth="27240" windowHeight="15560" activeTab="2" xr2:uid="{35824555-D2CA-254A-AC41-7E00E7980052}"/>
+    <workbookView xWindow="2420" yWindow="520" windowWidth="27240" windowHeight="15560" activeTab="2" xr2:uid="{35824555-D2CA-254A-AC41-7E00E7980052}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2296,7 +2296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{945E4251-CA6D-704A-ACF6-9BC71BB06730}">
   <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
working through days operational
</commit_message>
<xml_diff>
--- a/2014/OperationsDays2014_work.xlsx
+++ b/2014/OperationsDays2014_work.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elise/Desktop/MP/Belize-MP-Bruno-Boos/2014/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7697D4-2187-F143-8644-65593C70EFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147939CB-29A2-F942-925F-B90505F5FC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="520" windowWidth="27240" windowHeight="15560" activeTab="2" xr2:uid="{35824555-D2CA-254A-AC41-7E00E7980052}"/>
+    <workbookView xWindow="-32520" yWindow="3140" windowWidth="27240" windowHeight="15560" activeTab="2" xr2:uid="{35824555-D2CA-254A-AC41-7E00E7980052}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="104">
   <si>
     <t>401A</t>
   </si>
@@ -327,6 +327,30 @@
   </si>
   <si>
     <t>Date Removed</t>
+  </si>
+  <si>
+    <t>daysop according to data</t>
+  </si>
+  <si>
+    <t>402C</t>
+  </si>
+  <si>
+    <t>guessing this camera just saw nothing instead of wasn’t placed</t>
+  </si>
+  <si>
+    <t>402A</t>
+  </si>
+  <si>
+    <t>406F</t>
+  </si>
+  <si>
+    <t>This should be 0 because it malfunctioned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guessing this camera just saw nothing instead of wasn’t placed - was included in original analysis but I don’t know </t>
+  </si>
+  <si>
+    <t>in original data they just did 0's to the number of days even if the camera wasn't functional</t>
   </si>
 </sst>
 </file>
@@ -353,12 +377,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -373,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -381,6 +429,17 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2294,18 +2353,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{945E4251-CA6D-704A-ACF6-9BC71BB06730}">
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="6" width="17.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>82</v>
       </c>
@@ -2324,8 +2384,11 @@
       <c r="F1" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2344,28 +2407,37 @@
       <c r="F2" s="5">
         <v>41752</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="G2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="15">
         <v>0</v>
       </c>
-      <c r="C3">
-        <v>2014</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="16">
+        <v>2014</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="17">
         <v>41752</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="17">
         <v>41787</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="16">
+        <v>36</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -2384,8 +2456,11 @@
       <c r="F4" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -2404,8 +2479,11 @@
       <c r="F5" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
@@ -2424,53 +2502,44 @@
       <c r="F6" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="G7">
+        <v>37</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="12">
+        <v>52</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B9" s="3">
         <v>60</v>
-      </c>
-      <c r="C7">
-        <v>2014</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" s="5">
-        <v>41838</v>
-      </c>
-      <c r="F7" s="5">
-        <v>41900</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="3">
-        <v>40</v>
-      </c>
-      <c r="C8">
-        <v>2014</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" s="5">
-        <v>41900</v>
-      </c>
-      <c r="F8" s="5">
-        <v>41946</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="3">
-        <v>44</v>
       </c>
       <c r="C9">
         <v>2014</v>
@@ -2479,18 +2548,21 @@
         <v>71</v>
       </c>
       <c r="E9" s="5">
-        <v>41946</v>
+        <v>41838</v>
       </c>
       <c r="F9" s="5">
-        <v>41995</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>41900</v>
+      </c>
+      <c r="G9">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="B10" s="3">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C10">
         <v>2014</v>
@@ -2499,18 +2571,18 @@
         <v>71</v>
       </c>
       <c r="E10" s="5">
-        <v>41995</v>
+        <v>41900</v>
       </c>
       <c r="F10" s="5">
-        <v>42053</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="B11" s="3">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C11">
         <v>2014</v>
@@ -2519,18 +2591,18 @@
         <v>71</v>
       </c>
       <c r="E11" s="5">
-        <v>41716</v>
+        <v>41946</v>
       </c>
       <c r="F11" s="5">
-        <v>41752</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="B12" s="3">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C12">
         <v>2014</v>
@@ -2539,18 +2611,21 @@
         <v>71</v>
       </c>
       <c r="E12" s="5">
-        <v>41752</v>
+        <v>41995</v>
       </c>
       <c r="F12" s="5">
-        <v>41787</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>42053</v>
+      </c>
+      <c r="I12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="B13" s="3">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="C13">
         <v>2014</v>
@@ -2559,18 +2634,18 @@
         <v>71</v>
       </c>
       <c r="E13" s="5">
-        <v>41787</v>
+        <v>41716</v>
       </c>
       <c r="F13" s="5">
-        <v>41838</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>41752</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="B14" s="3">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>2014</v>
@@ -2579,18 +2654,18 @@
         <v>71</v>
       </c>
       <c r="E14" s="5">
-        <v>41838</v>
+        <v>41752</v>
       </c>
       <c r="F14" s="5">
-        <v>41900</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="3">
-        <v>44</v>
+        <v>19</v>
+      </c>
+      <c r="B15" s="7">
+        <v>60</v>
       </c>
       <c r="C15">
         <v>2014</v>
@@ -2599,98 +2674,98 @@
         <v>71</v>
       </c>
       <c r="E15" s="5">
-        <v>41900</v>
+        <v>41787</v>
       </c>
       <c r="F15" s="5">
-        <v>41946</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>41838</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="3">
-        <v>45</v>
+        <v>32</v>
+      </c>
+      <c r="B16" s="7">
+        <v>48</v>
       </c>
       <c r="C16">
         <v>2014</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E16" s="5">
-        <v>41946</v>
+        <v>41838</v>
       </c>
       <c r="F16" s="5">
-        <v>41995</v>
+        <v>41900</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="B17" s="3">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C17">
         <v>2014</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E17" s="5">
-        <v>41995</v>
+        <v>41900</v>
       </c>
       <c r="F17" s="5">
-        <v>42053</v>
+        <v>41946</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="B18" s="3">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C18">
         <v>2014</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="E18" s="5">
-        <v>41752</v>
+        <v>41946</v>
       </c>
       <c r="F18" s="5">
-        <v>41787</v>
+        <v>41995</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="B19" s="3">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="C19">
         <v>2014</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="E19" s="5">
-        <v>41787</v>
+        <v>41995</v>
       </c>
       <c r="F19" s="5">
-        <v>41838</v>
+        <v>42053</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="B20" s="3">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C20">
         <v>2014</v>
@@ -2699,18 +2774,18 @@
         <v>71</v>
       </c>
       <c r="E20" s="5">
-        <v>41838</v>
+        <v>41752</v>
       </c>
       <c r="F20" s="5">
-        <v>41900</v>
+        <v>41787</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="3">
-        <v>40</v>
+        <v>20</v>
+      </c>
+      <c r="B21" s="7">
+        <v>10</v>
       </c>
       <c r="C21">
         <v>2014</v>
@@ -2719,18 +2794,18 @@
         <v>71</v>
       </c>
       <c r="E21" s="5">
-        <v>41900</v>
+        <v>41787</v>
       </c>
       <c r="F21" s="5">
-        <v>41946</v>
+        <v>41838</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="3">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="B22" s="7">
+        <v>47</v>
       </c>
       <c r="C22">
         <v>2014</v>
@@ -2739,18 +2814,18 @@
         <v>71</v>
       </c>
       <c r="E22" s="5">
-        <v>41946</v>
+        <v>41838</v>
       </c>
       <c r="F22" s="5">
-        <v>41995</v>
+        <v>41900</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="B23" s="3">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C23">
         <v>2014</v>
@@ -2759,58 +2834,58 @@
         <v>71</v>
       </c>
       <c r="E23" s="5">
-        <v>41995</v>
+        <v>41900</v>
       </c>
       <c r="F23" s="5">
-        <v>42053</v>
+        <v>41946</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="B24" s="3">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C24">
         <v>2014</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E24" s="5">
-        <v>41716</v>
+        <v>41946</v>
       </c>
       <c r="F24" s="5">
-        <v>41752</v>
+        <v>41995</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="B25" s="3">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C25">
         <v>2014</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E25" s="5">
-        <v>41752</v>
+        <v>41995</v>
       </c>
       <c r="F25" s="5">
-        <v>41787</v>
+        <v>42053</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="B26" s="3">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C26">
         <v>2014</v>
@@ -2819,18 +2894,18 @@
         <v>80</v>
       </c>
       <c r="E26" s="5">
-        <v>41787</v>
+        <v>41716</v>
       </c>
       <c r="F26" s="5">
-        <v>41838</v>
+        <v>41752</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B27" s="3">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C27">
         <v>2014</v>
@@ -2839,18 +2914,18 @@
         <v>80</v>
       </c>
       <c r="E27" s="5">
-        <v>41838</v>
+        <v>41752</v>
       </c>
       <c r="F27" s="5">
-        <v>41900</v>
+        <v>41787</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="B28" s="3">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C28">
         <v>2014</v>
@@ -2859,18 +2934,18 @@
         <v>80</v>
       </c>
       <c r="E28" s="5">
-        <v>41900</v>
+        <v>41787</v>
       </c>
       <c r="F28" s="5">
-        <v>41946</v>
+        <v>41838</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B29" s="3">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="C29">
         <v>2014</v>
@@ -2879,38 +2954,38 @@
         <v>80</v>
       </c>
       <c r="E29" s="5">
-        <v>41946</v>
+        <v>41838</v>
       </c>
       <c r="F29" s="5">
-        <v>41995</v>
+        <v>41900</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="B30" s="3">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C30">
         <v>2014</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E30" s="5">
-        <v>41995</v>
+        <v>41900</v>
       </c>
       <c r="F30" s="5">
-        <v>42053</v>
+        <v>41946</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="B31" s="3">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C31">
         <v>2014</v>
@@ -2919,38 +2994,38 @@
         <v>80</v>
       </c>
       <c r="E31" s="5">
-        <v>41716</v>
+        <v>41946</v>
       </c>
       <c r="F31" s="5">
-        <v>41752</v>
+        <v>41995</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="B32" s="3">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C32">
         <v>2014</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E32" s="5">
-        <v>41752</v>
+        <v>41995</v>
       </c>
       <c r="F32" s="5">
-        <v>41787</v>
+        <v>42053</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B33" s="3">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C33">
         <v>2014</v>
@@ -2959,18 +3034,18 @@
         <v>80</v>
       </c>
       <c r="E33" s="5">
-        <v>41787</v>
+        <v>41716</v>
       </c>
       <c r="F33" s="5">
-        <v>41838</v>
+        <v>41752</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="3">
         <v>35</v>
-      </c>
-      <c r="B34" s="3">
-        <v>50</v>
       </c>
       <c r="C34">
         <v>2014</v>
@@ -2979,138 +3054,127 @@
         <v>80</v>
       </c>
       <c r="E34" s="5">
-        <v>41838</v>
+        <v>41752</v>
       </c>
       <c r="F34" s="5">
-        <v>41900</v>
+        <v>41787</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="B35" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C35">
         <v>2014</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E35" s="5">
-        <v>41900</v>
+        <v>41787</v>
       </c>
       <c r="F35" s="5">
-        <v>41946</v>
+        <v>41838</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="B36" s="3">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C36">
         <v>2014</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E36" s="5">
-        <v>41946</v>
+        <v>41838</v>
       </c>
       <c r="F36" s="5">
-        <v>41995</v>
+        <v>41900</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="B37" s="3">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C37">
         <v>2014</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E37" s="5">
-        <v>41716</v>
+        <v>41900</v>
       </c>
       <c r="F37" s="5">
-        <v>41752</v>
+        <v>41946</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="B38" s="3">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="C38">
         <v>2014</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E38" s="5">
-        <v>41752</v>
+        <v>41946</v>
       </c>
       <c r="F38" s="5">
-        <v>41787</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B39" s="3">
-        <v>45</v>
-      </c>
-      <c r="C39">
-        <v>2014</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E39" s="5">
-        <v>41787</v>
-      </c>
-      <c r="F39" s="5">
-        <v>41838</v>
-      </c>
+        <v>41995</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="B40" s="3">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C40">
         <v>2014</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E40" s="5">
-        <v>41838</v>
+        <v>41716</v>
       </c>
       <c r="F40" s="5">
-        <v>41900</v>
+        <v>41752</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="B41" s="3">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C41">
         <v>2014</v>
@@ -3119,15 +3183,15 @@
         <v>80</v>
       </c>
       <c r="E41" s="5">
-        <v>41900</v>
+        <v>41752</v>
       </c>
       <c r="F41" s="5">
-        <v>41946</v>
+        <v>41787</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="B42" s="3">
         <v>45</v>
@@ -3136,21 +3200,21 @@
         <v>2014</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E42" s="5">
-        <v>41946</v>
+        <v>41787</v>
       </c>
       <c r="F42" s="5">
-        <v>41995</v>
+        <v>41838</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="B43" s="3">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C43">
         <v>2014</v>
@@ -3159,18 +3223,18 @@
         <v>79</v>
       </c>
       <c r="E43" s="5">
-        <v>41995</v>
+        <v>41838</v>
       </c>
       <c r="F43" s="5">
-        <v>42053</v>
+        <v>41900</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="B44" s="3">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="C44">
         <v>2014</v>
@@ -3179,18 +3243,18 @@
         <v>80</v>
       </c>
       <c r="E44" s="5">
-        <v>41752</v>
+        <v>41900</v>
       </c>
       <c r="F44" s="5">
-        <v>41787</v>
+        <v>41946</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="B45" s="3">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C45">
         <v>2014</v>
@@ -3199,78 +3263,78 @@
         <v>80</v>
       </c>
       <c r="E45" s="5">
-        <v>41787</v>
+        <v>41946</v>
       </c>
       <c r="F45" s="5">
-        <v>41838</v>
+        <v>41995</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="B46" s="3">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C46">
         <v>2014</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E46" s="5">
-        <v>41838</v>
+        <v>41995</v>
       </c>
       <c r="F46" s="5">
-        <v>41900</v>
+        <v>42053</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="B47" s="3">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C47">
         <v>2014</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E47" s="5">
-        <v>41900</v>
+        <v>41752</v>
       </c>
       <c r="F47" s="5">
-        <v>41946</v>
+        <v>41787</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="B48" s="3">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C48">
         <v>2014</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E48" s="5">
-        <v>41946</v>
+        <v>41787</v>
       </c>
       <c r="F48" s="5">
-        <v>41995</v>
+        <v>41838</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="B49" s="3">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C49">
         <v>2014</v>
@@ -3279,38 +3343,38 @@
         <v>80</v>
       </c>
       <c r="E49" s="5">
-        <v>41716</v>
+        <v>41838</v>
       </c>
       <c r="F49" s="5">
-        <v>41752</v>
+        <v>41900</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="B50" s="3">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="C50">
         <v>2014</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E50" s="5">
-        <v>41752</v>
+        <v>41900</v>
       </c>
       <c r="F50" s="5">
-        <v>41787</v>
+        <v>41946</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="B51" s="3">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="C51">
         <v>2014</v>
@@ -3319,38 +3383,38 @@
         <v>79</v>
       </c>
       <c r="E51" s="5">
-        <v>41787</v>
+        <v>41946</v>
       </c>
       <c r="F51" s="5">
-        <v>41838</v>
+        <v>41995</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="B52" s="3">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="C52">
         <v>2014</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E52" s="5">
-        <v>41838</v>
+        <v>41716</v>
       </c>
       <c r="F52" s="5">
-        <v>41900</v>
+        <v>41752</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="B53" s="3">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C53">
         <v>2014</v>
@@ -3359,38 +3423,38 @@
         <v>80</v>
       </c>
       <c r="E53" s="5">
-        <v>41900</v>
+        <v>41752</v>
       </c>
       <c r="F53" s="5">
-        <v>41946</v>
+        <v>41787</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="B54" s="3">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="C54">
         <v>2014</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E54" s="5">
-        <v>41946</v>
+        <v>41787</v>
       </c>
       <c r="F54" s="5">
-        <v>41995</v>
+        <v>41838</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="B55" s="3">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="C55">
         <v>2014</v>
@@ -3399,18 +3463,18 @@
         <v>79</v>
       </c>
       <c r="E55" s="5">
-        <v>41995</v>
+        <v>41838</v>
       </c>
       <c r="F55" s="5">
-        <v>42053</v>
+        <v>41900</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="B56" s="3">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C56">
         <v>2014</v>
@@ -3419,18 +3483,18 @@
         <v>80</v>
       </c>
       <c r="E56" s="5">
-        <v>41716</v>
+        <v>41900</v>
       </c>
       <c r="F56" s="5">
-        <v>41752</v>
+        <v>41946</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="B57" s="3">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="C57">
         <v>2014</v>
@@ -3439,18 +3503,18 @@
         <v>80</v>
       </c>
       <c r="E57" s="5">
-        <v>41752</v>
+        <v>41946</v>
       </c>
       <c r="F57" s="5">
-        <v>41787</v>
+        <v>41995</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="B58" s="3">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="C58">
         <v>2014</v>
@@ -3459,98 +3523,98 @@
         <v>79</v>
       </c>
       <c r="E58" s="5">
-        <v>41787</v>
+        <v>41995</v>
       </c>
       <c r="F58" s="5">
-        <v>41838</v>
+        <v>42053</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="B59" s="3">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C59">
         <v>2014</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E59" s="5">
-        <v>41838</v>
+        <v>41716</v>
       </c>
       <c r="F59" s="5">
-        <v>41900</v>
+        <v>41752</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="3">
+        <v>35</v>
+      </c>
+      <c r="C60">
+        <v>2014</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E60" s="5">
+        <v>41752</v>
+      </c>
+      <c r="F60" s="5">
+        <v>41787</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B61" s="9">
         <v>50</v>
       </c>
-      <c r="B60" s="3">
-        <v>44</v>
-      </c>
-      <c r="C60">
-        <v>2014</v>
-      </c>
-      <c r="D60" s="3" t="s">
+      <c r="C61">
+        <v>2014</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E60" s="5">
-        <v>41900</v>
-      </c>
-      <c r="F60" s="5">
-        <v>41946</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B61" s="3">
-        <v>35</v>
-      </c>
-      <c r="C61">
-        <v>2014</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="E61" s="5">
-        <v>41752</v>
+        <v>41787</v>
       </c>
       <c r="F61" s="5">
-        <v>41787</v>
+        <v>41838</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B62" s="3">
+      <c r="A62" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B62" s="9">
         <v>48</v>
       </c>
       <c r="C62">
         <v>2014</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E62" s="5">
-        <v>41787</v>
+        <v>41838</v>
       </c>
       <c r="F62" s="5">
-        <v>41838</v>
+        <v>41900</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="B63" s="3">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C63">
         <v>2014</v>
@@ -3559,15 +3623,15 @@
         <v>79</v>
       </c>
       <c r="E63" s="5">
-        <v>41995</v>
+        <v>41900</v>
       </c>
       <c r="F63" s="5">
-        <v>42053</v>
+        <v>41946</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B64" s="3">
         <v>35</v>
@@ -3587,7 +3651,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B65" s="3">
         <v>48</v>
@@ -3607,30 +3671,30 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="B66" s="3">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C66">
         <v>2014</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E66" s="5">
-        <v>41900</v>
+        <v>41995</v>
       </c>
       <c r="F66" s="5">
-        <v>41946</v>
+        <v>42053</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="s">
-        <v>61</v>
+      <c r="A67" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="B67" s="3">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C67">
         <v>2014</v>
@@ -3639,15 +3703,15 @@
         <v>80</v>
       </c>
       <c r="E67" s="5">
-        <v>41946</v>
+        <v>41752</v>
       </c>
       <c r="F67" s="5">
-        <v>41995</v>
+        <v>41787</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B68" s="3">
         <v>48</v>
@@ -3656,7 +3720,7 @@
         <v>2014</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E68" s="5">
         <v>41787</v>
@@ -3667,50 +3731,50 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B69" s="3">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C69">
         <v>2014</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E69" s="5">
-        <v>41838</v>
+        <v>41900</v>
       </c>
       <c r="F69" s="5">
-        <v>41900</v>
+        <v>41946</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B70" s="3">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="C70">
         <v>2014</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E70" s="5">
-        <v>41900</v>
+        <v>41946</v>
       </c>
       <c r="F70" s="5">
-        <v>41946</v>
+        <v>41995</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="B71" s="3">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C71">
         <v>2014</v>
@@ -3719,18 +3783,18 @@
         <v>71</v>
       </c>
       <c r="E71" s="5">
-        <v>41946</v>
+        <v>41787</v>
       </c>
       <c r="F71" s="5">
-        <v>41995</v>
+        <v>41838</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="B72" s="3">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C72">
         <v>2014</v>
@@ -3739,9 +3803,69 @@
         <v>71</v>
       </c>
       <c r="E72" s="5">
+        <v>41838</v>
+      </c>
+      <c r="F72" s="5">
+        <v>41900</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B73" s="3">
+        <v>44</v>
+      </c>
+      <c r="C73">
+        <v>2014</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E73" s="5">
+        <v>41900</v>
+      </c>
+      <c r="F73" s="5">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B74" s="3">
+        <v>35</v>
+      </c>
+      <c r="C74">
+        <v>2014</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E74" s="5">
+        <v>41946</v>
+      </c>
+      <c r="F74" s="5">
         <v>41995</v>
       </c>
-      <c r="F72" s="5">
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B75" s="3">
+        <v>47</v>
+      </c>
+      <c r="C75">
+        <v>2014</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E75" s="5">
+        <v>41995</v>
+      </c>
+      <c r="F75" s="5">
         <v>42053</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Went through 2014 to pull together cam locations - data for 2017 northing and eastings were flipped so fixed that too. Deleted old shapefile
</commit_message>
<xml_diff>
--- a/2014/OperationsDays2014_work.xlsx
+++ b/2014/OperationsDays2014_work.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elise/Desktop/MP/Belize-MP-Bruno-Boos/2014/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147939CB-29A2-F942-925F-B90505F5FC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D6BC58-35D8-7C4D-B780-86AE1D665AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32520" yWindow="3140" windowWidth="27240" windowHeight="15560" activeTab="2" xr2:uid="{35824555-D2CA-254A-AC41-7E00E7980052}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26300" windowHeight="16520" activeTab="5" xr2:uid="{35824555-D2CA-254A-AC41-7E00E7980052}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="OperationsDays2014" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
+    <sheet name="FINAL" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="113">
   <si>
     <t>401A</t>
   </si>
@@ -351,15 +352,43 @@
   </si>
   <si>
     <t>in original data they just did 0's to the number of days even if the camera wasn't functional</t>
+  </si>
+  <si>
+    <t>Easting</t>
+  </si>
+  <si>
+    <t>Northing</t>
+  </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>Lon</t>
+  </si>
+  <si>
+    <t>408F</t>
+  </si>
+  <si>
+    <t>Functioning?</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>IDK</t>
+  </si>
+  <si>
+    <t>Days</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="0.00000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -377,7 +406,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -408,6 +437,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -421,7 +462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -440,6 +481,18 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2355,8 +2408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{945E4251-CA6D-704A-ACF6-9BC71BB06730}">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2785,7 +2838,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="7">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="C21">
         <v>2014</v>
@@ -2805,7 +2858,7 @@
         <v>33</v>
       </c>
       <c r="B22" s="7">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="C22">
         <v>2014</v>
@@ -3879,7 +3932,7 @@
   <dimension ref="A1:C72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C72"/>
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4689,19 +4742,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{505DB0B9-E048-0A4F-958B-1599B5D3CFCF}">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="37.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -4714,8 +4769,10 @@
       <c r="D1" s="5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4728,8 +4785,13 @@
       <c r="D2" s="5">
         <v>41752</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G2" s="1"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -4742,8 +4804,13 @@
       <c r="D3" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G3" s="1"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -4756,8 +4823,13 @@
       <c r="D4" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G4" s="1"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -4770,11 +4842,14 @@
       <c r="D5" s="5">
         <v>41900</v>
       </c>
-      <c r="E5" s="6">
-        <v>41900</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" s="6"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
@@ -4787,8 +4862,13 @@
       <c r="D6" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G6" s="1"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -4801,8 +4881,13 @@
       <c r="D7" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G7" s="1"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
@@ -4815,8 +4900,13 @@
       <c r="D8" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G8" s="1"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>53</v>
       </c>
@@ -4829,8 +4919,13 @@
       <c r="D9" s="5">
         <v>41995</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G9" s="1"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>63</v>
       </c>
@@ -4843,8 +4938,13 @@
       <c r="D10" s="5">
         <v>42053</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G10" s="1"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -4857,8 +4957,13 @@
       <c r="D11" s="5">
         <v>41752</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G11" s="1"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -4871,8 +4976,13 @@
       <c r="D12" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G12" s="1"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -4885,8 +4995,13 @@
       <c r="D13" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G13" s="1"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
@@ -4899,8 +5014,13 @@
       <c r="D14" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G14" s="1"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -4913,8 +5033,13 @@
       <c r="D15" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G15" s="1"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>54</v>
       </c>
@@ -4927,8 +5052,13 @@
       <c r="D16" s="5">
         <v>41995</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G16" s="1"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>64</v>
       </c>
@@ -4941,8 +5071,13 @@
       <c r="D17" s="5">
         <v>42053</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G17" s="1"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -4955,8 +5090,13 @@
       <c r="D18" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G18" s="1"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -4969,8 +5109,13 @@
       <c r="D19" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G19" s="1"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
@@ -4983,8 +5128,13 @@
       <c r="D20" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G20" s="1"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
@@ -4997,8 +5147,13 @@
       <c r="D21" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G21" s="1"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
@@ -5011,8 +5166,13 @@
       <c r="D22" s="5">
         <v>41995</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G22" s="1"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>65</v>
       </c>
@@ -5025,8 +5185,13 @@
       <c r="D23" s="5">
         <v>42053</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G23" s="1"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -5039,8 +5204,13 @@
       <c r="D24" s="5">
         <v>41752</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G24" s="1"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
@@ -5053,8 +5223,13 @@
       <c r="D25" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G25" s="1"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -5067,8 +5242,13 @@
       <c r="D26" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G26" s="1"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
@@ -5081,8 +5261,13 @@
       <c r="D27" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G27" s="1"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>45</v>
       </c>
@@ -5095,8 +5280,13 @@
       <c r="D28" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G28" s="1"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
@@ -5109,8 +5299,13 @@
       <c r="D29" s="5">
         <v>41995</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G29" s="1"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>66</v>
       </c>
@@ -5123,8 +5318,13 @@
       <c r="D30" s="5">
         <v>42053</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G30" s="1"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -5137,8 +5337,13 @@
       <c r="D31" s="5">
         <v>41752</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G31" s="1"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>11</v>
       </c>
@@ -5151,8 +5356,13 @@
       <c r="D32" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G32" s="1"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>22</v>
       </c>
@@ -5165,8 +5375,13 @@
       <c r="D33" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G33" s="1"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
@@ -5179,8 +5394,13 @@
       <c r="D34" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G34" s="1"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>46</v>
       </c>
@@ -5193,8 +5413,13 @@
       <c r="D35" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G35" s="1"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>57</v>
       </c>
@@ -5207,8 +5432,13 @@
       <c r="D36" s="5">
         <v>41995</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G36" s="1"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>4</v>
       </c>
@@ -5221,8 +5451,13 @@
       <c r="D37" s="5">
         <v>41752</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G37" s="1"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>12</v>
       </c>
@@ -5235,8 +5470,13 @@
       <c r="D38" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G38" s="1"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>23</v>
       </c>
@@ -5249,8 +5489,13 @@
       <c r="D39" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G39" s="1"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>36</v>
       </c>
@@ -5263,8 +5508,13 @@
       <c r="D40" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G40" s="1"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>47</v>
       </c>
@@ -5277,8 +5527,13 @@
       <c r="D41" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G41" s="1"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>58</v>
       </c>
@@ -5291,8 +5546,13 @@
       <c r="D42" s="5">
         <v>41995</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G42" s="1"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>67</v>
       </c>
@@ -5305,8 +5565,13 @@
       <c r="D43" s="5">
         <v>42053</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G43" s="1"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="18"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>13</v>
       </c>
@@ -5319,8 +5584,13 @@
       <c r="D44" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G44" s="1"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>24</v>
       </c>
@@ -5333,8 +5603,13 @@
       <c r="D45" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G45" s="1"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>37</v>
       </c>
@@ -5347,8 +5622,13 @@
       <c r="D46" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G46" s="1"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="19"/>
+      <c r="K46" s="19"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
@@ -5361,8 +5641,13 @@
       <c r="D47" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G47" s="1"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="19"/>
+      <c r="K47" s="19"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>59</v>
       </c>
@@ -5375,8 +5660,13 @@
       <c r="D48" s="5">
         <v>41995</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G48" s="1"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="19"/>
+      <c r="K48" s="19"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>5</v>
       </c>
@@ -5389,8 +5679,13 @@
       <c r="D49" s="5">
         <v>41752</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G49" s="1"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="19"/>
+      <c r="K49" s="19"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>14</v>
       </c>
@@ -5403,8 +5698,13 @@
       <c r="D50" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G50" s="1"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>25</v>
       </c>
@@ -5417,8 +5717,13 @@
       <c r="D51" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G51" s="1"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="19"/>
+      <c r="K51" s="19"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>38</v>
       </c>
@@ -5431,8 +5736,13 @@
       <c r="D52" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G52" s="1"/>
+      <c r="H52" s="18"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="19"/>
+      <c r="K52" s="19"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>49</v>
       </c>
@@ -5445,8 +5755,13 @@
       <c r="D53" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G53" s="1"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="19"/>
+      <c r="K53" s="19"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>60</v>
       </c>
@@ -5459,8 +5774,13 @@
       <c r="D54" s="5">
         <v>41995</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G54" s="1"/>
+      <c r="H54" s="18"/>
+      <c r="I54" s="18"/>
+      <c r="J54" s="19"/>
+      <c r="K54" s="19"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>68</v>
       </c>
@@ -5473,8 +5793,13 @@
       <c r="D55" s="5">
         <v>42053</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G55" s="1"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="18"/>
+      <c r="J55" s="19"/>
+      <c r="K55" s="19"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>6</v>
       </c>
@@ -5487,8 +5812,13 @@
       <c r="D56" s="5">
         <v>41752</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G56" s="1"/>
+      <c r="H56" s="18"/>
+      <c r="I56" s="18"/>
+      <c r="J56" s="19"/>
+      <c r="K56" s="19"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>15</v>
       </c>
@@ -5501,8 +5831,13 @@
       <c r="D57" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G57" s="1"/>
+      <c r="H57" s="18"/>
+      <c r="I57" s="18"/>
+      <c r="J57" s="19"/>
+      <c r="K57" s="19"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>26</v>
       </c>
@@ -5515,8 +5850,13 @@
       <c r="D58" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G58" s="1"/>
+      <c r="H58" s="18"/>
+      <c r="I58" s="18"/>
+      <c r="J58" s="19"/>
+      <c r="K58" s="19"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>39</v>
       </c>
@@ -5529,8 +5869,13 @@
       <c r="D59" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G59" s="1"/>
+      <c r="H59" s="18"/>
+      <c r="I59" s="18"/>
+      <c r="J59" s="19"/>
+      <c r="K59" s="19"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>50</v>
       </c>
@@ -5543,8 +5888,13 @@
       <c r="D60" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G60" s="1"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="18"/>
+      <c r="J60" s="19"/>
+      <c r="K60" s="19"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -5557,8 +5907,13 @@
       <c r="D61" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G61" s="1"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
+      <c r="J61" s="19"/>
+      <c r="K61" s="19"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>27</v>
       </c>
@@ -5571,8 +5926,13 @@
       <c r="D62" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G62" s="1"/>
+      <c r="H62" s="18"/>
+      <c r="I62" s="18"/>
+      <c r="J62" s="19"/>
+      <c r="K62" s="19"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>69</v>
       </c>
@@ -5585,8 +5945,13 @@
       <c r="D63" s="5">
         <v>42053</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G63" s="1"/>
+      <c r="H63" s="18"/>
+      <c r="I63" s="18"/>
+      <c r="J63" s="19"/>
+      <c r="K63" s="19"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>17</v>
       </c>
@@ -5599,8 +5964,13 @@
       <c r="D64" s="5">
         <v>41787</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G64" s="1"/>
+      <c r="H64" s="18"/>
+      <c r="I64" s="18"/>
+      <c r="J64" s="19"/>
+      <c r="K64" s="19"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>28</v>
       </c>
@@ -5613,8 +5983,12 @@
       <c r="D65" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H65" s="18"/>
+      <c r="I65" s="18"/>
+      <c r="J65" s="19"/>
+      <c r="K65" s="19"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>51</v>
       </c>
@@ -5627,8 +6001,13 @@
       <c r="D66" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G66" s="1"/>
+      <c r="H66" s="18"/>
+      <c r="I66" s="18"/>
+      <c r="J66" s="19"/>
+      <c r="K66" s="19"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>61</v>
       </c>
@@ -5641,8 +6020,13 @@
       <c r="D67" s="5">
         <v>41995</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G67" s="1"/>
+      <c r="H67" s="18"/>
+      <c r="I67" s="18"/>
+      <c r="J67" s="19"/>
+      <c r="K67" s="19"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>29</v>
       </c>
@@ -5655,8 +6039,12 @@
       <c r="D68" s="5">
         <v>41838</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H68" s="18"/>
+      <c r="I68" s="18"/>
+      <c r="J68" s="19"/>
+      <c r="K68" s="19"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>40</v>
       </c>
@@ -5669,8 +6057,13 @@
       <c r="D69" s="5">
         <v>41900</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G69" s="1"/>
+      <c r="H69" s="18"/>
+      <c r="I69" s="18"/>
+      <c r="J69" s="19"/>
+      <c r="K69" s="19"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>52</v>
       </c>
@@ -5683,8 +6076,13 @@
       <c r="D70" s="5">
         <v>41946</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G70" s="1"/>
+      <c r="H70" s="18"/>
+      <c r="I70" s="18"/>
+      <c r="J70" s="19"/>
+      <c r="K70" s="19"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>62</v>
       </c>
@@ -5697,8 +6095,13 @@
       <c r="D71" s="5">
         <v>41995</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G71" s="1"/>
+      <c r="H71" s="18"/>
+      <c r="I71" s="18"/>
+      <c r="J71" s="19"/>
+      <c r="K71" s="19"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>70</v>
       </c>
@@ -5711,6 +6114,39 @@
       <c r="D72" s="5">
         <v>42053</v>
       </c>
+      <c r="G72" s="1"/>
+      <c r="H72" s="18"/>
+      <c r="I72" s="18"/>
+      <c r="J72" s="19"/>
+      <c r="K72" s="19"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G73" s="1"/>
+      <c r="H73" s="18"/>
+      <c r="I73" s="18"/>
+      <c r="J73" s="19"/>
+      <c r="K73" s="19"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G74" s="1"/>
+      <c r="H74" s="18"/>
+      <c r="I74" s="18"/>
+      <c r="J74" s="19"/>
+      <c r="K74" s="19"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G75" s="1"/>
+      <c r="H75" s="18"/>
+      <c r="I75" s="18"/>
+      <c r="J75" s="19"/>
+      <c r="K75" s="19"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G76" s="1"/>
+      <c r="H76" s="18"/>
+      <c r="I76" s="18"/>
+      <c r="J76" s="19"/>
+      <c r="K76" s="19"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D72">
@@ -5718,4 +6154,2251 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AFE9C49-45FC-1B41-898C-D4CBEEC367A8}">
+  <dimension ref="A1:J76"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="18">
+        <v>299504.905195</v>
+      </c>
+      <c r="C2" s="18">
+        <v>1927436.73594</v>
+      </c>
+      <c r="D2" s="19">
+        <v>17.4257174219</v>
+      </c>
+      <c r="E2" s="19">
+        <v>-88.887561237900002</v>
+      </c>
+      <c r="G2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="4">
+        <v>41716</v>
+      </c>
+      <c r="I2" s="5">
+        <v>41752</v>
+      </c>
+      <c r="J2" s="3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="25">
+        <v>306056.17661090998</v>
+      </c>
+      <c r="C3" s="25">
+        <v>1928108.4087691901</v>
+      </c>
+      <c r="D3" s="26">
+        <v>17.432360270499998</v>
+      </c>
+      <c r="E3" s="26">
+        <v>-88.825965892799999</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="G3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" s="4">
+        <v>41752</v>
+      </c>
+      <c r="I3" s="5">
+        <v>41787</v>
+      </c>
+      <c r="J3" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="18">
+        <v>306148.48781801999</v>
+      </c>
+      <c r="C4" s="18">
+        <v>1928078.52171337</v>
+      </c>
+      <c r="D4" s="19">
+        <v>17.4320982168</v>
+      </c>
+      <c r="E4" s="19">
+        <v>-88.825094397699999</v>
+      </c>
+      <c r="G4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H4" s="4">
+        <v>41787</v>
+      </c>
+      <c r="I4" s="5">
+        <v>41838</v>
+      </c>
+      <c r="J4" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="18">
+        <v>305786.260633</v>
+      </c>
+      <c r="C5" s="18">
+        <v>1928483.08558</v>
+      </c>
+      <c r="D5" s="19">
+        <v>17.435722001599999</v>
+      </c>
+      <c r="E5" s="19">
+        <v>-88.828540000000004</v>
+      </c>
+      <c r="G5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" s="4">
+        <v>41838</v>
+      </c>
+      <c r="I5" s="5">
+        <v>41900</v>
+      </c>
+      <c r="J5" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="18">
+        <v>305786.260633</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1928483.08558</v>
+      </c>
+      <c r="D6" s="19">
+        <v>17.435722001599999</v>
+      </c>
+      <c r="E6" s="19">
+        <v>-88.828540000000004</v>
+      </c>
+      <c r="G6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" s="4">
+        <v>41900</v>
+      </c>
+      <c r="I6" s="5">
+        <v>41946</v>
+      </c>
+      <c r="J6" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="21">
+        <v>300194.58872699999</v>
+      </c>
+      <c r="C7" s="21">
+        <v>1927401.1617999999</v>
+      </c>
+      <c r="D7" s="22">
+        <v>17.425457420600001</v>
+      </c>
+      <c r="E7" s="22">
+        <v>-88.881067267000006</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="G7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H7" s="4">
+        <v>41716</v>
+      </c>
+      <c r="I7" s="5">
+        <v>41752</v>
+      </c>
+      <c r="J7" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="21">
+        <v>303763.51611725002</v>
+      </c>
+      <c r="C8" s="21">
+        <v>1927657.2376085899</v>
+      </c>
+      <c r="D8" s="22">
+        <v>17.4280852017</v>
+      </c>
+      <c r="E8" s="22">
+        <v>-88.847502665899995</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H8" s="4">
+        <v>41787</v>
+      </c>
+      <c r="I8" s="5">
+        <v>41838</v>
+      </c>
+      <c r="J8" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="18">
+        <v>303877.52769000002</v>
+      </c>
+      <c r="C9" s="18">
+        <v>1927198.7547299999</v>
+      </c>
+      <c r="D9" s="19">
+        <v>17.423953001699999</v>
+      </c>
+      <c r="E9" s="19">
+        <v>-88.846387999900003</v>
+      </c>
+      <c r="G9" t="s">
+        <v>91</v>
+      </c>
+      <c r="H9" s="4">
+        <v>41838</v>
+      </c>
+      <c r="I9" s="5">
+        <v>41900</v>
+      </c>
+      <c r="J9" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="18">
+        <v>303877.52769000002</v>
+      </c>
+      <c r="C10" s="18">
+        <v>1927198.7547299999</v>
+      </c>
+      <c r="D10" s="19">
+        <v>17.423953001699999</v>
+      </c>
+      <c r="E10" s="19">
+        <v>-88.846387999900003</v>
+      </c>
+      <c r="G10" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" s="4">
+        <v>41900</v>
+      </c>
+      <c r="I10" s="5">
+        <v>41946</v>
+      </c>
+      <c r="J10" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="18">
+        <v>303759.676553</v>
+      </c>
+      <c r="C11" s="18">
+        <v>1927582.42793</v>
+      </c>
+      <c r="D11" s="19">
+        <v>17.427409001600001</v>
+      </c>
+      <c r="E11" s="19">
+        <v>-88.847531999899999</v>
+      </c>
+      <c r="G11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H11" s="4">
+        <v>41946</v>
+      </c>
+      <c r="I11" s="5">
+        <v>41995</v>
+      </c>
+      <c r="J11" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="18">
+        <v>303762.064182</v>
+      </c>
+      <c r="C12" s="18">
+        <v>1927587.60717</v>
+      </c>
+      <c r="D12" s="19">
+        <v>17.4274560016</v>
+      </c>
+      <c r="E12" s="19">
+        <v>-88.847509999899998</v>
+      </c>
+      <c r="G12" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" t="s">
+        <v>93</v>
+      </c>
+      <c r="I12" s="5">
+        <v>42053</v>
+      </c>
+      <c r="J12" s="3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="18">
+        <v>291031.29713800002</v>
+      </c>
+      <c r="C13" s="18">
+        <v>1926154.1713099999</v>
+      </c>
+      <c r="D13" s="19">
+        <v>17.4133595138</v>
+      </c>
+      <c r="E13" s="19">
+        <v>-88.967180888000001</v>
+      </c>
+      <c r="G13" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" s="4">
+        <v>41716</v>
+      </c>
+      <c r="I13" s="5">
+        <v>41752</v>
+      </c>
+      <c r="J13" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="18">
+        <v>291227.26662695</v>
+      </c>
+      <c r="C14" s="18">
+        <v>1926257.0645459001</v>
+      </c>
+      <c r="D14" s="19">
+        <v>17.4143072239</v>
+      </c>
+      <c r="E14" s="19">
+        <v>-88.965346756499997</v>
+      </c>
+      <c r="G14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" s="4">
+        <v>41752</v>
+      </c>
+      <c r="I14" s="5">
+        <v>41787</v>
+      </c>
+      <c r="J14" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="18">
+        <v>290976.16779005999</v>
+      </c>
+      <c r="C15" s="18">
+        <v>1926510.2484219701</v>
+      </c>
+      <c r="D15" s="19">
+        <v>17.416571136200002</v>
+      </c>
+      <c r="E15" s="19">
+        <v>-88.9677341079</v>
+      </c>
+      <c r="G15" t="s">
+        <v>91</v>
+      </c>
+      <c r="H15" s="4">
+        <v>41787</v>
+      </c>
+      <c r="I15" s="5">
+        <v>41838</v>
+      </c>
+      <c r="J15" s="7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="18">
+        <v>290967.02983199997</v>
+      </c>
+      <c r="C16" s="18">
+        <v>1926302.5530399999</v>
+      </c>
+      <c r="D16" s="19">
+        <v>17.414694001600001</v>
+      </c>
+      <c r="E16" s="19">
+        <v>-88.967799999999997</v>
+      </c>
+      <c r="G16" t="s">
+        <v>91</v>
+      </c>
+      <c r="H16" s="4">
+        <v>41838</v>
+      </c>
+      <c r="I16" s="5">
+        <v>41900</v>
+      </c>
+      <c r="J16" s="7">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="18">
+        <v>290967.02983199997</v>
+      </c>
+      <c r="C17" s="18">
+        <v>1926302.5530399999</v>
+      </c>
+      <c r="D17" s="19">
+        <v>17.414694001600001</v>
+      </c>
+      <c r="E17" s="19">
+        <v>-88.967799999999997</v>
+      </c>
+      <c r="G17" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" s="4">
+        <v>41900</v>
+      </c>
+      <c r="I17" s="5">
+        <v>41946</v>
+      </c>
+      <c r="J17" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="18">
+        <v>287303.29920499999</v>
+      </c>
+      <c r="C18" s="18">
+        <v>1935282.1670899999</v>
+      </c>
+      <c r="D18" s="19">
+        <v>17.4954690016</v>
+      </c>
+      <c r="E18" s="19">
+        <v>-89.003162000000003</v>
+      </c>
+      <c r="G18" t="s">
+        <v>91</v>
+      </c>
+      <c r="H18" s="4">
+        <v>41946</v>
+      </c>
+      <c r="I18" s="5">
+        <v>41995</v>
+      </c>
+      <c r="J18" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="18">
+        <v>291689.06010800001</v>
+      </c>
+      <c r="C19" s="18">
+        <v>1929549.2330499999</v>
+      </c>
+      <c r="D19" s="19">
+        <v>17.4440910016</v>
+      </c>
+      <c r="E19" s="19">
+        <v>-88.961318999900001</v>
+      </c>
+      <c r="G19" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" t="s">
+        <v>93</v>
+      </c>
+      <c r="I19" s="5">
+        <v>42053</v>
+      </c>
+      <c r="J19" s="3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="18">
+        <v>305818.49404684</v>
+      </c>
+      <c r="C20" s="18">
+        <v>1928442.1680182901</v>
+      </c>
+      <c r="D20" s="19">
+        <v>17.435355115299998</v>
+      </c>
+      <c r="E20" s="19">
+        <v>-88.828232938900001</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H20" s="4">
+        <v>41752</v>
+      </c>
+      <c r="I20" s="5">
+        <v>41787</v>
+      </c>
+      <c r="J20" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="18">
+        <v>304607.04380715999</v>
+      </c>
+      <c r="C21" s="18">
+        <v>1927908.1141007501</v>
+      </c>
+      <c r="D21" s="19">
+        <v>17.430425208700001</v>
+      </c>
+      <c r="E21" s="19">
+        <v>-88.839586571500007</v>
+      </c>
+      <c r="G21" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" s="4">
+        <v>41787</v>
+      </c>
+      <c r="I21" s="5">
+        <v>41838</v>
+      </c>
+      <c r="J21" s="7">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="18">
+        <v>304744.39105199999</v>
+      </c>
+      <c r="C22" s="18">
+        <v>1927455.8324800001</v>
+      </c>
+      <c r="D22" s="19">
+        <v>17.426351001600001</v>
+      </c>
+      <c r="E22" s="19">
+        <v>-88.838252999900007</v>
+      </c>
+      <c r="G22" t="s">
+        <v>92</v>
+      </c>
+      <c r="H22" s="4">
+        <v>41838</v>
+      </c>
+      <c r="I22" s="5">
+        <v>41900</v>
+      </c>
+      <c r="J22" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="18">
+        <v>304744.39105199999</v>
+      </c>
+      <c r="C23" s="18">
+        <v>1927455.8324800001</v>
+      </c>
+      <c r="D23" s="19">
+        <v>17.426351001600001</v>
+      </c>
+      <c r="E23" s="19">
+        <v>-88.838252999900007</v>
+      </c>
+      <c r="G23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H23" s="4">
+        <v>41900</v>
+      </c>
+      <c r="I23" s="5">
+        <v>41946</v>
+      </c>
+      <c r="J23" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="18">
+        <v>304653.30888600001</v>
+      </c>
+      <c r="C24" s="18">
+        <v>1927840.23786</v>
+      </c>
+      <c r="D24" s="19">
+        <v>17.429816001599999</v>
+      </c>
+      <c r="E24" s="19">
+        <v>-88.8391449999</v>
+      </c>
+      <c r="G24" t="s">
+        <v>92</v>
+      </c>
+      <c r="H24" s="4">
+        <v>41946</v>
+      </c>
+      <c r="I24" s="5">
+        <v>41995</v>
+      </c>
+      <c r="J24" s="3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="18">
+        <v>304653.30888600001</v>
+      </c>
+      <c r="C25" s="18">
+        <v>1927840.23786</v>
+      </c>
+      <c r="D25" s="19">
+        <v>17.429816001599999</v>
+      </c>
+      <c r="E25" s="19">
+        <v>-88.8391449999</v>
+      </c>
+      <c r="G25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H25" t="s">
+        <v>93</v>
+      </c>
+      <c r="I25" s="5">
+        <v>42053</v>
+      </c>
+      <c r="J25" s="3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="18">
+        <v>283422.79744300002</v>
+      </c>
+      <c r="C26" s="18">
+        <v>1932759.10038</v>
+      </c>
+      <c r="D26" s="19">
+        <v>17.4723052571</v>
+      </c>
+      <c r="E26" s="19">
+        <v>-89.039438539900004</v>
+      </c>
+      <c r="G26" t="s">
+        <v>90</v>
+      </c>
+      <c r="H26" s="4">
+        <v>41716</v>
+      </c>
+      <c r="I26" s="5">
+        <v>41752</v>
+      </c>
+      <c r="J26" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="18">
+        <v>283453.94751376001</v>
+      </c>
+      <c r="C27" s="18">
+        <v>1932032.7170178399</v>
+      </c>
+      <c r="D27" s="19">
+        <v>17.465746560900001</v>
+      </c>
+      <c r="E27" s="19">
+        <v>-89.039072264599994</v>
+      </c>
+      <c r="G27" t="s">
+        <v>90</v>
+      </c>
+      <c r="H27" s="4">
+        <v>41752</v>
+      </c>
+      <c r="I27" s="5">
+        <v>41787</v>
+      </c>
+      <c r="J27" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="18">
+        <v>283405.80972992</v>
+      </c>
+      <c r="C28" s="18">
+        <v>1933797.7603963399</v>
+      </c>
+      <c r="D28" s="19">
+        <v>17.481686227099999</v>
+      </c>
+      <c r="E28" s="19">
+        <v>-89.039703002899998</v>
+      </c>
+      <c r="G28" t="s">
+        <v>90</v>
+      </c>
+      <c r="H28" s="4">
+        <v>41787</v>
+      </c>
+      <c r="I28" s="5">
+        <v>41838</v>
+      </c>
+      <c r="J28" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="18">
+        <v>283565.37313899997</v>
+      </c>
+      <c r="C29" s="18">
+        <v>1934622.18707</v>
+      </c>
+      <c r="D29" s="19">
+        <v>17.489149001600001</v>
+      </c>
+      <c r="E29" s="19">
+        <v>-89.038284000000004</v>
+      </c>
+      <c r="G29" t="s">
+        <v>90</v>
+      </c>
+      <c r="H29" s="4">
+        <v>41838</v>
+      </c>
+      <c r="I29" s="5">
+        <v>41900</v>
+      </c>
+      <c r="J29" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="18">
+        <v>283565.37313899997</v>
+      </c>
+      <c r="C30" s="18">
+        <v>1934622.18707</v>
+      </c>
+      <c r="D30" s="19">
+        <v>17.489149001600001</v>
+      </c>
+      <c r="E30" s="19">
+        <v>-89.038284000000004</v>
+      </c>
+      <c r="G30" t="s">
+        <v>90</v>
+      </c>
+      <c r="H30" s="4">
+        <v>41900</v>
+      </c>
+      <c r="I30" s="5">
+        <v>41946</v>
+      </c>
+      <c r="J30" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="18">
+        <v>283532.99642799998</v>
+      </c>
+      <c r="C31" s="18">
+        <v>1933998.625</v>
+      </c>
+      <c r="D31" s="19">
+        <v>17.483513001599999</v>
+      </c>
+      <c r="E31" s="19">
+        <v>-89.038526000000005</v>
+      </c>
+      <c r="G31" t="s">
+        <v>90</v>
+      </c>
+      <c r="H31" s="4">
+        <v>41946</v>
+      </c>
+      <c r="I31" s="5">
+        <v>41995</v>
+      </c>
+      <c r="J31" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="18">
+        <v>285409.15846399998</v>
+      </c>
+      <c r="C32" s="18">
+        <v>1935699.1400299999</v>
+      </c>
+      <c r="D32" s="19">
+        <v>17.499055001599999</v>
+      </c>
+      <c r="E32" s="19">
+        <v>-89.021034999999998</v>
+      </c>
+      <c r="G32" t="s">
+        <v>90</v>
+      </c>
+      <c r="H32" t="s">
+        <v>93</v>
+      </c>
+      <c r="I32" s="5">
+        <v>42053</v>
+      </c>
+      <c r="J32" s="3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="18">
+        <v>283348.02513099997</v>
+      </c>
+      <c r="C33" s="18">
+        <v>1933227.82889</v>
+      </c>
+      <c r="D33" s="19">
+        <v>17.476532237000001</v>
+      </c>
+      <c r="E33" s="19">
+        <v>-89.040189534700005</v>
+      </c>
+      <c r="G33" t="s">
+        <v>91</v>
+      </c>
+      <c r="H33" s="4">
+        <v>41716</v>
+      </c>
+      <c r="I33" s="5">
+        <v>41752</v>
+      </c>
+      <c r="J33" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="18">
+        <v>283558.40077482001</v>
+      </c>
+      <c r="C34" s="18">
+        <v>1934171.3291649499</v>
+      </c>
+      <c r="D34" s="19">
+        <v>17.4850755579</v>
+      </c>
+      <c r="E34" s="19">
+        <v>-89.038304246699994</v>
+      </c>
+      <c r="G34" t="s">
+        <v>91</v>
+      </c>
+      <c r="H34" s="4">
+        <v>41752</v>
+      </c>
+      <c r="I34" s="5">
+        <v>41787</v>
+      </c>
+      <c r="J34" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="18">
+        <v>283359.16892055998</v>
+      </c>
+      <c r="C35" s="18">
+        <v>1934194.56842823</v>
+      </c>
+      <c r="D35" s="19">
+        <v>17.485266233400001</v>
+      </c>
+      <c r="E35" s="19">
+        <v>-89.040182010300001</v>
+      </c>
+      <c r="G35" t="s">
+        <v>91</v>
+      </c>
+      <c r="H35" s="4">
+        <v>41787</v>
+      </c>
+      <c r="I35" s="5">
+        <v>41838</v>
+      </c>
+      <c r="J35" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="18">
+        <v>292119.81952600001</v>
+      </c>
+      <c r="C36" s="18">
+        <v>1930183.3022700001</v>
+      </c>
+      <c r="D36" s="19">
+        <v>17.4498590016</v>
+      </c>
+      <c r="E36" s="19">
+        <v>-88.957325999899993</v>
+      </c>
+      <c r="G36" t="s">
+        <v>91</v>
+      </c>
+      <c r="H36" s="4">
+        <v>41838</v>
+      </c>
+      <c r="I36" s="5">
+        <v>41900</v>
+      </c>
+      <c r="J36" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="18">
+        <v>292119.81952600001</v>
+      </c>
+      <c r="C37" s="18">
+        <v>1930183.3022700001</v>
+      </c>
+      <c r="D37" s="19">
+        <v>17.4498590016</v>
+      </c>
+      <c r="E37" s="19">
+        <v>-88.957325999899993</v>
+      </c>
+      <c r="G37" t="s">
+        <v>91</v>
+      </c>
+      <c r="H37" s="4">
+        <v>41900</v>
+      </c>
+      <c r="I37" s="5">
+        <v>41946</v>
+      </c>
+      <c r="J37" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" s="18">
+        <v>286926.279767</v>
+      </c>
+      <c r="C38" s="18">
+        <v>1935340.0449300001</v>
+      </c>
+      <c r="D38" s="19">
+        <v>17.4959560016</v>
+      </c>
+      <c r="E38" s="19">
+        <v>-89.006716999999995</v>
+      </c>
+      <c r="G38" t="s">
+        <v>91</v>
+      </c>
+      <c r="H38" s="4">
+        <v>41946</v>
+      </c>
+      <c r="I38" s="5">
+        <v>41995</v>
+      </c>
+      <c r="J38" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B39" s="21">
+        <v>291882.85421999998</v>
+      </c>
+      <c r="C39" s="21">
+        <v>1929921.28217</v>
+      </c>
+      <c r="D39" s="22">
+        <v>17.447470001599999</v>
+      </c>
+      <c r="E39" s="22">
+        <v>-88.959530999999998</v>
+      </c>
+      <c r="F39" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="G39" t="s">
+        <v>91</v>
+      </c>
+      <c r="H39" t="s">
+        <v>93</v>
+      </c>
+      <c r="I39" s="5">
+        <v>42053</v>
+      </c>
+      <c r="J39" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="18">
+        <v>282835.17592100002</v>
+      </c>
+      <c r="C40" s="18">
+        <v>1934016.5273200001</v>
+      </c>
+      <c r="D40" s="19">
+        <v>17.483607204599998</v>
+      </c>
+      <c r="E40" s="19">
+        <v>-89.045096509700002</v>
+      </c>
+      <c r="G40" t="s">
+        <v>91</v>
+      </c>
+      <c r="H40" s="4">
+        <v>41716</v>
+      </c>
+      <c r="I40" s="5">
+        <v>41752</v>
+      </c>
+      <c r="J40" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="18">
+        <v>282356.32871541003</v>
+      </c>
+      <c r="C41" s="18">
+        <v>1934100.6435211401</v>
+      </c>
+      <c r="D41" s="19">
+        <v>17.4843205982</v>
+      </c>
+      <c r="E41" s="19">
+        <v>-89.049612479100006</v>
+      </c>
+      <c r="G41" t="s">
+        <v>91</v>
+      </c>
+      <c r="H41" s="4">
+        <v>41752</v>
+      </c>
+      <c r="I41" s="5">
+        <v>41787</v>
+      </c>
+      <c r="J41" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" s="18">
+        <v>287745.44159881002</v>
+      </c>
+      <c r="C42" s="18">
+        <v>1932108.8227268099</v>
+      </c>
+      <c r="D42" s="19">
+        <v>17.466844216599998</v>
+      </c>
+      <c r="E42" s="19">
+        <v>-88.9986865021</v>
+      </c>
+      <c r="G42" t="s">
+        <v>91</v>
+      </c>
+      <c r="H42" s="4">
+        <v>41787</v>
+      </c>
+      <c r="I42" s="5">
+        <v>41838</v>
+      </c>
+      <c r="J42" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" s="18">
+        <v>283443.887155</v>
+      </c>
+      <c r="C43" s="18">
+        <v>1934824.6298700001</v>
+      </c>
+      <c r="D43" s="19">
+        <v>17.4909660016</v>
+      </c>
+      <c r="E43" s="19">
+        <v>-89.039447999999993</v>
+      </c>
+      <c r="G43" t="s">
+        <v>91</v>
+      </c>
+      <c r="H43" s="4">
+        <v>41838</v>
+      </c>
+      <c r="I43" s="5">
+        <v>41900</v>
+      </c>
+      <c r="J43" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="18">
+        <v>283443.887155</v>
+      </c>
+      <c r="C44" s="18">
+        <v>1934824.6298700001</v>
+      </c>
+      <c r="D44" s="19">
+        <v>17.4909660016</v>
+      </c>
+      <c r="E44" s="19">
+        <v>-89.039447999999993</v>
+      </c>
+      <c r="G44" t="s">
+        <v>91</v>
+      </c>
+      <c r="H44" s="4">
+        <v>41900</v>
+      </c>
+      <c r="I44" s="5">
+        <v>41946</v>
+      </c>
+      <c r="J44" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" s="18">
+        <v>284554.38671599998</v>
+      </c>
+      <c r="C45" s="18">
+        <v>1935261.5530300001</v>
+      </c>
+      <c r="D45" s="19">
+        <v>17.4950200016</v>
+      </c>
+      <c r="E45" s="19">
+        <v>-89.029038</v>
+      </c>
+      <c r="G45" t="s">
+        <v>91</v>
+      </c>
+      <c r="H45" s="4">
+        <v>41946</v>
+      </c>
+      <c r="I45" s="5">
+        <v>41995</v>
+      </c>
+      <c r="J45" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" s="18">
+        <v>288174.65701000002</v>
+      </c>
+      <c r="C46" s="18">
+        <v>1935951.49031</v>
+      </c>
+      <c r="D46" s="19">
+        <v>17.5015980015</v>
+      </c>
+      <c r="E46" s="19">
+        <v>-88.995024999899996</v>
+      </c>
+      <c r="G46" t="s">
+        <v>91</v>
+      </c>
+      <c r="H46" t="s">
+        <v>93</v>
+      </c>
+      <c r="I46" s="5">
+        <v>42053</v>
+      </c>
+      <c r="J46" s="3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" s="18">
+        <v>284005.43206953001</v>
+      </c>
+      <c r="C47" s="18">
+        <v>1935106.3507042199</v>
+      </c>
+      <c r="D47" s="19">
+        <v>17.493565117100001</v>
+      </c>
+      <c r="E47" s="19">
+        <v>-89.034190161300003</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H47" s="4">
+        <v>41752</v>
+      </c>
+      <c r="I47" s="5">
+        <v>41787</v>
+      </c>
+      <c r="J47" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" s="18">
+        <v>283343.92635382002</v>
+      </c>
+      <c r="C48" s="18">
+        <v>1933425.36076947</v>
+      </c>
+      <c r="D48" s="19">
+        <v>17.478316220699998</v>
+      </c>
+      <c r="E48" s="19">
+        <v>-89.040248008000006</v>
+      </c>
+      <c r="G48" t="s">
+        <v>92</v>
+      </c>
+      <c r="H48" s="4">
+        <v>41787</v>
+      </c>
+      <c r="I48" s="5">
+        <v>41838</v>
+      </c>
+      <c r="J48" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" s="18">
+        <v>291804.87758799997</v>
+      </c>
+      <c r="C49" s="18">
+        <v>1929880.9037299999</v>
+      </c>
+      <c r="D49" s="19">
+        <v>17.447098001600001</v>
+      </c>
+      <c r="E49" s="19">
+        <v>-88.960261000000003</v>
+      </c>
+      <c r="G49" t="s">
+        <v>92</v>
+      </c>
+      <c r="H49" s="4">
+        <v>41838</v>
+      </c>
+      <c r="I49" s="5">
+        <v>41900</v>
+      </c>
+      <c r="J49" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" s="18">
+        <v>291804.87758799997</v>
+      </c>
+      <c r="C50" s="18">
+        <v>1929880.9037299999</v>
+      </c>
+      <c r="D50" s="19">
+        <v>17.447098001600001</v>
+      </c>
+      <c r="E50" s="19">
+        <v>-88.960261000000003</v>
+      </c>
+      <c r="G50" t="s">
+        <v>92</v>
+      </c>
+      <c r="H50" s="4">
+        <v>41900</v>
+      </c>
+      <c r="I50" s="5">
+        <v>41946</v>
+      </c>
+      <c r="J50" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="18">
+        <v>287878.57947</v>
+      </c>
+      <c r="C51" s="18">
+        <v>1931465.91285</v>
+      </c>
+      <c r="D51" s="19">
+        <v>17.461049001599999</v>
+      </c>
+      <c r="E51" s="19">
+        <v>-88.997370000000004</v>
+      </c>
+      <c r="G51" t="s">
+        <v>92</v>
+      </c>
+      <c r="H51" s="4">
+        <v>41946</v>
+      </c>
+      <c r="I51" s="5">
+        <v>41995</v>
+      </c>
+      <c r="J51" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B52" s="21">
+        <v>287876.78542299999</v>
+      </c>
+      <c r="C52" s="21">
+        <v>1931477.22276</v>
+      </c>
+      <c r="D52" s="22">
+        <v>17.461151001600001</v>
+      </c>
+      <c r="E52" s="22">
+        <v>-88.997388000000001</v>
+      </c>
+      <c r="F52" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="G52" t="s">
+        <v>92</v>
+      </c>
+      <c r="H52" t="s">
+        <v>93</v>
+      </c>
+      <c r="I52" s="5">
+        <v>42053</v>
+      </c>
+      <c r="J52" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="18">
+        <v>283361.81445499999</v>
+      </c>
+      <c r="C53" s="18">
+        <v>1934000.2571099999</v>
+      </c>
+      <c r="D53" s="19">
+        <v>17.483511203100001</v>
+      </c>
+      <c r="E53" s="19">
+        <v>-89.040137531799999</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H53" s="28">
+        <v>41716</v>
+      </c>
+      <c r="I53" s="29">
+        <v>41752</v>
+      </c>
+      <c r="J53" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" s="18">
+        <v>283089.78155140998</v>
+      </c>
+      <c r="C54" s="18">
+        <v>1934100.5194174701</v>
+      </c>
+      <c r="D54" s="19">
+        <v>17.484390593899999</v>
+      </c>
+      <c r="E54" s="19">
+        <v>-89.042708337199997</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H54" s="28">
+        <v>41752</v>
+      </c>
+      <c r="I54" s="29">
+        <v>41787</v>
+      </c>
+      <c r="J54" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" s="18">
+        <v>287509.22436975001</v>
+      </c>
+      <c r="C55" s="18">
+        <v>1932206.27708486</v>
+      </c>
+      <c r="D55" s="19">
+        <v>17.467702217300001</v>
+      </c>
+      <c r="E55" s="19">
+        <v>-89.000919529399994</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H55" s="28">
+        <v>41787</v>
+      </c>
+      <c r="I55" s="29">
+        <v>41838</v>
+      </c>
+      <c r="J55" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B56" s="18">
+        <v>283207.63169299997</v>
+      </c>
+      <c r="C56" s="18">
+        <v>1934953.4694099999</v>
+      </c>
+      <c r="D56" s="19">
+        <v>17.492107001600001</v>
+      </c>
+      <c r="E56" s="19">
+        <v>-89.041685000000001</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H56" s="28">
+        <v>41838</v>
+      </c>
+      <c r="I56" s="29">
+        <v>41900</v>
+      </c>
+      <c r="J56" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B57" s="18">
+        <v>283207.63169299997</v>
+      </c>
+      <c r="C57" s="18">
+        <v>1934953.4694099999</v>
+      </c>
+      <c r="D57" s="19">
+        <v>17.492107001600001</v>
+      </c>
+      <c r="E57" s="19">
+        <v>-89.041685000000001</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H57" s="28">
+        <v>41900</v>
+      </c>
+      <c r="I57" s="29">
+        <v>41946</v>
+      </c>
+      <c r="J57" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="18">
+        <v>283847.44533900003</v>
+      </c>
+      <c r="C58" s="18">
+        <v>1934963.11839</v>
+      </c>
+      <c r="D58" s="19">
+        <v>17.492256001600001</v>
+      </c>
+      <c r="E58" s="19">
+        <v>-89.035663</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H58" s="28">
+        <v>41946</v>
+      </c>
+      <c r="I58" s="29">
+        <v>41995</v>
+      </c>
+      <c r="J58" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B59" s="18">
+        <v>290370.82823599997</v>
+      </c>
+      <c r="C59" s="18">
+        <v>1936481.31121</v>
+      </c>
+      <c r="D59" s="19">
+        <v>17.5065910016</v>
+      </c>
+      <c r="E59" s="19">
+        <v>-88.974401</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H59" t="s">
+        <v>93</v>
+      </c>
+      <c r="I59" s="29">
+        <v>42053</v>
+      </c>
+      <c r="J59" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" s="18">
+        <v>282533.28121699998</v>
+      </c>
+      <c r="C60" s="18">
+        <v>1934008.6982799999</v>
+      </c>
+      <c r="D60" s="19">
+        <v>17.483507206300001</v>
+      </c>
+      <c r="E60" s="19">
+        <v>-89.047937497000007</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H60" s="28">
+        <v>41716</v>
+      </c>
+      <c r="I60" s="29">
+        <v>41752</v>
+      </c>
+      <c r="J60" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B61" s="18">
+        <v>282303.57875599997</v>
+      </c>
+      <c r="C61" s="18">
+        <v>1934085.4919803501</v>
+      </c>
+      <c r="D61" s="19">
+        <v>17.4841786056</v>
+      </c>
+      <c r="E61" s="19">
+        <v>-89.050107489200002</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H61" s="28">
+        <v>41752</v>
+      </c>
+      <c r="I61" s="29">
+        <v>41787</v>
+      </c>
+      <c r="J61" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" s="18">
+        <v>286611.75533861999</v>
+      </c>
+      <c r="C62" s="18">
+        <v>1934360.05185166</v>
+      </c>
+      <c r="D62" s="19">
+        <v>17.4870732493</v>
+      </c>
+      <c r="E62" s="19">
+        <v>-89.009580642200007</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H62" s="28">
+        <v>41787</v>
+      </c>
+      <c r="I62" s="29">
+        <v>41838</v>
+      </c>
+      <c r="J62" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B63" s="18">
+        <v>291398.27318999998</v>
+      </c>
+      <c r="C63" s="18">
+        <v>1929086.41557</v>
+      </c>
+      <c r="D63" s="19">
+        <v>17.439883001599998</v>
+      </c>
+      <c r="E63" s="19">
+        <v>-88.964010999899998</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H63" s="28">
+        <v>41838</v>
+      </c>
+      <c r="I63" s="29">
+        <v>41900</v>
+      </c>
+      <c r="J63" s="9">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B64" s="18">
+        <v>291398.27318999998</v>
+      </c>
+      <c r="C64" s="18">
+        <v>1929086.41557</v>
+      </c>
+      <c r="D64" s="19">
+        <v>17.439883001599998</v>
+      </c>
+      <c r="E64" s="19">
+        <v>-88.964010999899998</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H64" s="28">
+        <v>41900</v>
+      </c>
+      <c r="I64" s="29">
+        <v>41946</v>
+      </c>
+      <c r="J64" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>16</v>
+      </c>
+      <c r="B65" s="18">
+        <v>283544.13810902002</v>
+      </c>
+      <c r="C65" s="18">
+        <v>1931474.4064891599</v>
+      </c>
+      <c r="D65" s="19">
+        <v>17.460711822099999</v>
+      </c>
+      <c r="E65" s="19">
+        <v>-89.038167246499995</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H65" s="28">
+        <v>41752</v>
+      </c>
+      <c r="I65" s="29">
+        <v>41787</v>
+      </c>
+      <c r="J65" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B66" s="18">
+        <v>283393.20614977001</v>
+      </c>
+      <c r="C66" s="18">
+        <v>1933215.38778182</v>
+      </c>
+      <c r="D66" s="19">
+        <v>17.476424217400002</v>
+      </c>
+      <c r="E66" s="19">
+        <v>-89.039763001300003</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H66" s="28">
+        <v>41787</v>
+      </c>
+      <c r="I66" s="29">
+        <v>41838</v>
+      </c>
+      <c r="J66" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B67" s="18">
+        <v>291693.76281599997</v>
+      </c>
+      <c r="C67" s="18">
+        <v>1928982.5379999999</v>
+      </c>
+      <c r="D67" s="19">
+        <v>17.4389720016</v>
+      </c>
+      <c r="E67" s="19">
+        <v>-88.961219999899996</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H67" t="s">
+        <v>93</v>
+      </c>
+      <c r="I67" s="29">
+        <v>42053</v>
+      </c>
+      <c r="J67" s="3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>17</v>
+      </c>
+      <c r="B68" s="18">
+        <v>283420.20895781001</v>
+      </c>
+      <c r="C68" s="18">
+        <v>1931719.0368985101</v>
+      </c>
+      <c r="D68" s="19">
+        <v>17.4629097081</v>
+      </c>
+      <c r="E68" s="19">
+        <v>-89.039358270799994</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H68" s="28">
+        <v>41752</v>
+      </c>
+      <c r="I68" s="29">
+        <v>41787</v>
+      </c>
+      <c r="J68" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B69" s="18">
+        <v>282700.78485583997</v>
+      </c>
+      <c r="C69" s="18">
+        <v>1934209.8173727</v>
+      </c>
+      <c r="D69" s="19">
+        <v>17.485340230999999</v>
+      </c>
+      <c r="E69" s="19">
+        <v>-89.046381085099995</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H69" s="28">
+        <v>41787</v>
+      </c>
+      <c r="I69" s="29">
+        <v>41838</v>
+      </c>
+      <c r="J69" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B70" s="18">
+        <v>283343.072109</v>
+      </c>
+      <c r="C70" s="18">
+        <v>1933216.34296</v>
+      </c>
+      <c r="D70" s="19">
+        <v>17.476428001599999</v>
+      </c>
+      <c r="E70" s="19">
+        <v>-89.040234999999996</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H70" s="28">
+        <v>41900</v>
+      </c>
+      <c r="I70" s="29">
+        <v>41946</v>
+      </c>
+      <c r="J70" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B71" s="18">
+        <v>283383.91773699998</v>
+      </c>
+      <c r="C71" s="18">
+        <v>1933012.4384600001</v>
+      </c>
+      <c r="D71" s="19">
+        <v>17.474590001599999</v>
+      </c>
+      <c r="E71" s="19">
+        <v>-89.039829999999995</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H71" s="28">
+        <v>41946</v>
+      </c>
+      <c r="I71" s="29">
+        <v>41995</v>
+      </c>
+      <c r="J71" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B72" s="18">
+        <v>302853.88205802999</v>
+      </c>
+      <c r="C72" s="18">
+        <v>1927593.5446202001</v>
+      </c>
+      <c r="D72" s="19">
+        <v>17.427430197500001</v>
+      </c>
+      <c r="E72" s="19">
+        <v>-88.856057768599996</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H72" s="28">
+        <v>41787</v>
+      </c>
+      <c r="I72" s="29">
+        <v>41838</v>
+      </c>
+      <c r="J72" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B73" s="18">
+        <v>302849.58338500001</v>
+      </c>
+      <c r="C73" s="18">
+        <v>1927087.38922</v>
+      </c>
+      <c r="D73" s="19">
+        <v>17.422857001600001</v>
+      </c>
+      <c r="E73" s="19">
+        <v>-88.856051999900004</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H73" s="28">
+        <v>41838</v>
+      </c>
+      <c r="I73" s="29">
+        <v>41900</v>
+      </c>
+      <c r="J73" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B74" s="18">
+        <v>302849.58338500001</v>
+      </c>
+      <c r="C74" s="18">
+        <v>1927087.38922</v>
+      </c>
+      <c r="D74" s="19">
+        <v>17.422857001600001</v>
+      </c>
+      <c r="E74" s="19">
+        <v>-88.856051999900004</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H74" s="28">
+        <v>41900</v>
+      </c>
+      <c r="I74" s="29">
+        <v>41946</v>
+      </c>
+      <c r="J74" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B75" s="18">
+        <v>305716.08936300001</v>
+      </c>
+      <c r="C75" s="18">
+        <v>1928611.3781900001</v>
+      </c>
+      <c r="D75" s="19">
+        <v>17.436875001600001</v>
+      </c>
+      <c r="E75" s="19">
+        <v>-88.829211999899996</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H75" s="28">
+        <v>41946</v>
+      </c>
+      <c r="I75" s="29">
+        <v>41995</v>
+      </c>
+      <c r="J75" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B76" s="18">
+        <v>305715.87476899999</v>
+      </c>
+      <c r="C76" s="18">
+        <v>1928611.1588699999</v>
+      </c>
+      <c r="D76" s="19">
+        <v>17.436873001599999</v>
+      </c>
+      <c r="E76" s="19">
+        <v>-88.829213999900006</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H76" t="s">
+        <v>93</v>
+      </c>
+      <c r="I76" s="29">
+        <v>42053</v>
+      </c>
+      <c r="J76" s="3">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E76">
+    <sortCondition ref="A2:A76"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>